<commit_message>
* Update test plans * Working win logic * More responsive design :)
</commit_message>
<xml_diff>
--- a/Project 02/Web Tech Test Plan.xlsx
+++ b/Project 02/Web Tech Test Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aef782b26370319e/School Documents/2021 Fall/CIS 435-002/Projects/project2/Project 02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{E03DC43A-6366-44E8-9ED3-ACA789DF0ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11B5D03F-57AC-467C-91FB-6318F67A6428}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{E03DC43A-6366-44E8-9ED3-ACA789DF0ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E29F836-C36B-4875-8747-F69FD60121C8}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="16395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="43">
   <si>
     <t>Test case plan</t>
   </si>
@@ -140,6 +140,24 @@
   </si>
   <si>
     <t>Player always plays with "x"</t>
+  </si>
+  <si>
+    <t>Wins on Diagonal are counted appropriately</t>
+  </si>
+  <si>
+    <t>Nope! They should not wrap around, it'll always cross center in a 3x3 grid.</t>
+  </si>
+  <si>
+    <t>Player does not always start first</t>
+  </si>
+  <si>
+    <t>Player cannot place a piece when the CPU is playing</t>
+  </si>
+  <si>
+    <t>Player cannot place a piece in an already occupied cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No deadlocks happen from the CPU :) </t>
   </si>
 </sst>
 </file>
@@ -656,8 +674,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -666,7 +684,7 @@
     <col min="2" max="2" width="30.1328125" customWidth="1"/>
     <col min="3" max="3" width="29.19921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.1328125" customWidth="1"/>
+    <col min="5" max="5" width="29.86328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.59765625" customWidth="1"/>
     <col min="7" max="7" width="16.3984375" customWidth="1"/>
     <col min="8" max="8" width="15.1328125" customWidth="1"/>
@@ -874,24 +892,45 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="4:4" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="4:5" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D17" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="4:4" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="19" spans="4:4" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="20" spans="4:4" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="21" spans="4:4" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="22" spans="4:4" s="4" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="4:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="4:5" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D19" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D20" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5" s="2" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D21" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5" s="4" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D22" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="4:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="4:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="25" spans="4:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="26" spans="4:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="24" spans="4:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="25" spans="4:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="26" spans="4:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:I1"/>

</xml_diff>